<commit_message>
Fixes BAS for enlisted members
</commit_message>
<xml_diff>
--- a/Air_Force_money.xlsx
+++ b/Air_Force_money.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Money Projections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Money Projections\AF Finance Projector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB7B928-ADC3-4DB6-B698-5CD57174FA79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4369FC23-6AEC-4B72-8DF6-C96D393ECD3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="1188" windowWidth="17868" windowHeight="10926" activeTab="2" xr2:uid="{23D836E6-1353-4D7A-B5B7-85954EF3EBD8}"/>
+    <workbookView xWindow="702" yWindow="648" windowWidth="10656" windowHeight="10926" activeTab="2" xr2:uid="{23D836E6-1353-4D7A-B5B7-85954EF3EBD8}"/>
   </bookViews>
   <sheets>
     <sheet name="BAS" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -118,10 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,16 +441,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -456,20 +458,21 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>256</v>
+      <c r="B2" s="1">
+        <v>256.68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>310</v>
+      <c r="B3" s="1">
+        <v>372.71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -625,7 +628,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -639,10 +642,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>6000</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>19500</v>
       </c>
     </row>

</xml_diff>